<commit_message>
fix: use sqlite custom funtion to solve the problem of sqlite not supporting regex
</commit_message>
<xml_diff>
--- a/test_data/multi_table_data.xlsx
+++ b/test_data/multi_table_data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myprj\validatelite\test_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245F0CDD-80EF-4928-BDB0-0AE5B990F270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21960" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21960" windowHeight="13176" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -173,11 +167,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,7 +249,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -562,14 +556,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="3" max="3" width="19.5546875" customWidth="1"/>
@@ -577,7 +571,7 @@
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +591,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -617,7 +611,7 @@
         <v>19690223</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -637,7 +631,7 @@
         <v>19680231</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -657,7 +651,7 @@
         <v>19690223</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -677,7 +671,7 @@
         <v>19692323</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.6" customHeight="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -697,7 +691,7 @@
         <v>19690223</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.6" customHeight="1">
       <c r="A7">
         <v>6</v>
       </c>
@@ -717,7 +711,7 @@
         <v>19690224</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.6" customHeight="1">
       <c r="A8">
         <v>7</v>
       </c>
@@ -740,22 +734,31 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" xr:uid="{FE3C29D7-4080-43E2-8253-455260AACB34}"/>
-    <hyperlink ref="C8" r:id="rId2" xr:uid="{33BF121E-03E5-4FD8-A732-2CD94924BCCD}"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -772,7 +775,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>100</v>
       </c>
@@ -789,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>200</v>
       </c>
@@ -806,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>300</v>
       </c>
@@ -823,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>400</v>
       </c>
@@ -831,7 +834,7 @@
         <v>28</v>
       </c>
       <c r="C5">
-        <v>299.99</v>
+        <v>299.89999999999998</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -840,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>500</v>
       </c>
@@ -864,19 +867,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -893,7 +896,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -910,7 +913,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -927,7 +930,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -944,7 +947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -961,7 +964,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -972,7 +975,7 @@
         <v>45296</v>
       </c>
       <c r="D6">
-        <v>89.99</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
feat: Implement DATE_FORMAT validation support for SQLite and PostgreSQL databases
</commit_message>
<xml_diff>
--- a/test_data/multi_table_data.xlsx
+++ b/test_data/multi_table_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21960" windowHeight="13176" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21960" windowHeight="13176" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -161,6 +161,52 @@
   </si>
   <si>
     <t>yangyang@gmail.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>03/04/2004</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>23/04/2007</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>02/31/2008</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>03/24/2006</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/07/2005</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:33:44</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:33:46</t>
+  </si>
+  <si>
+    <t>12:33:47</t>
+  </si>
+  <si>
+    <t>12:33:78</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>25:33:48</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -244,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -254,6 +300,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -560,7 +607,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -745,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -868,18 +915,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -895,8 +944,14 @@
       <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -912,8 +967,14 @@
       <c r="E2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -929,8 +990,14 @@
       <c r="E3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -946,8 +1013,14 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -963,8 +1036,14 @@
       <c r="E5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -979,10 +1058,17 @@
       </c>
       <c r="E6" t="s">
         <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>